<commit_message>
AOI plots + new study
</commit_message>
<xml_diff>
--- a/studies/2020_Aperol_Git/coding data/data/manual_coding_MandSE_diagrams.xlsx
+++ b/studies/2020_Aperol_Git/coding data/data/manual_coding_MandSE_diagrams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\EmpSchul\Forschung_Projekte&amp;Studien\01 PROJECTS\2020_MK_GK_CL_APEROL\Behavioral coding\manual coding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\studies\2020_Aperol_Git\coding data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C2B93C-FAB6-46B3-A37B-2B305077C3D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8772" xr2:uid="{D9BE113E-CD22-4B9F-8AEA-F1B95AFAE5BC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8772" xr2:uid="{D9BE113E-CD22-4B9F-8AEA-F1B95AFAE5BC}"/>
   </bookViews>
   <sheets>
     <sheet name="manual_coding_withseconds" sheetId="1" r:id="rId1"/>
@@ -1555,7 +1555,7 @@
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1617,7 +1617,7 @@
         <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
@@ -6072,9 +6072,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DD2F59-5577-4BF1-9B09-7232E83E7D11}">
   <dimension ref="A1:AM75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P130" sqref="P130"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>

</xml_diff>